<commit_message>
Data update for past 3 days
</commit_message>
<xml_diff>
--- a/coronadata_age_sex.xlsx
+++ b/coronadata_age_sex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvisc\Desktop\coronadata-local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A297455-3DF1-4693-B5AB-15D6D88FAE25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A55510-08C6-416B-922E-DE833683F4AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -949,11 +949,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y66"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U82" sqref="U82"/>
+      <selection pane="bottomLeft" activeCell="V79" sqref="V79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6063,6 +6063,249 @@
         <v>61.165048543689316</v>
       </c>
     </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>43974</v>
+      </c>
+      <c r="B67">
+        <v>43</v>
+      </c>
+      <c r="C67">
+        <v>69</v>
+      </c>
+      <c r="D67">
+        <v>107</v>
+      </c>
+      <c r="E67">
+        <v>261</v>
+      </c>
+      <c r="F67">
+        <v>135</v>
+      </c>
+      <c r="G67">
+        <v>234</v>
+      </c>
+      <c r="H67">
+        <v>109</v>
+      </c>
+      <c r="I67">
+        <v>189</v>
+      </c>
+      <c r="J67">
+        <v>156</v>
+      </c>
+      <c r="K67">
+        <v>225</v>
+      </c>
+      <c r="L67">
+        <v>167</v>
+      </c>
+      <c r="M67">
+        <v>182</v>
+      </c>
+      <c r="N67">
+        <v>147</v>
+      </c>
+      <c r="O67">
+        <v>177</v>
+      </c>
+      <c r="P67">
+        <v>103</v>
+      </c>
+      <c r="Q67">
+        <v>146</v>
+      </c>
+      <c r="R67">
+        <v>46</v>
+      </c>
+      <c r="S67">
+        <v>121</v>
+      </c>
+      <c r="T67">
+        <v>3</v>
+      </c>
+      <c r="U67">
+        <v>7</v>
+      </c>
+      <c r="V67">
+        <f t="shared" ref="V67" si="5">SUM(B67,D67,F67,H67,J67,L67,N67,P67,R67,T67)</f>
+        <v>1016</v>
+      </c>
+      <c r="W67">
+        <f t="shared" ref="W67" si="6">SUM(C67,E67,G67,I67,K67,M67,O67,Q67,S67,U67)</f>
+        <v>1611</v>
+      </c>
+      <c r="X67">
+        <f>(V67/(V67+W67))*100</f>
+        <v>38.675295013323179</v>
+      </c>
+      <c r="Y67">
+        <f>(W67/(V67+W67))*100</f>
+        <v>61.324704986676814</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B68">
+        <v>43</v>
+      </c>
+      <c r="C68">
+        <v>69</v>
+      </c>
+      <c r="D68">
+        <v>107</v>
+      </c>
+      <c r="E68">
+        <v>268</v>
+      </c>
+      <c r="F68">
+        <v>136</v>
+      </c>
+      <c r="G68">
+        <v>236</v>
+      </c>
+      <c r="H68">
+        <v>109</v>
+      </c>
+      <c r="I68">
+        <v>190</v>
+      </c>
+      <c r="J68">
+        <v>157</v>
+      </c>
+      <c r="K68">
+        <v>226</v>
+      </c>
+      <c r="L68">
+        <v>168</v>
+      </c>
+      <c r="M68">
+        <v>183</v>
+      </c>
+      <c r="N68">
+        <v>147</v>
+      </c>
+      <c r="O68">
+        <v>178</v>
+      </c>
+      <c r="P68">
+        <v>105</v>
+      </c>
+      <c r="Q68">
+        <v>147</v>
+      </c>
+      <c r="R68">
+        <v>47</v>
+      </c>
+      <c r="S68">
+        <v>122</v>
+      </c>
+      <c r="T68">
+        <v>3</v>
+      </c>
+      <c r="U68">
+        <v>7</v>
+      </c>
+      <c r="V68">
+        <f t="shared" ref="V68" si="7">SUM(B68,D68,F68,H68,J68,L68,N68,P68,R68,T68)</f>
+        <v>1022</v>
+      </c>
+      <c r="W68">
+        <f t="shared" ref="W68" si="8">SUM(C68,E68,G68,I68,K68,M68,O68,Q68,S68,U68)</f>
+        <v>1626</v>
+      </c>
+      <c r="X68">
+        <f>(V68/(V68+W68))*100</f>
+        <v>38.59516616314199</v>
+      </c>
+      <c r="Y68">
+        <f>(W68/(V68+W68))*100</f>
+        <v>61.40483383685801</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B69">
+        <v>44</v>
+      </c>
+      <c r="C69">
+        <v>69</v>
+      </c>
+      <c r="D69">
+        <v>109</v>
+      </c>
+      <c r="E69">
+        <v>272</v>
+      </c>
+      <c r="F69">
+        <v>136</v>
+      </c>
+      <c r="G69">
+        <v>240</v>
+      </c>
+      <c r="H69">
+        <v>111</v>
+      </c>
+      <c r="I69">
+        <v>192</v>
+      </c>
+      <c r="J69">
+        <v>158</v>
+      </c>
+      <c r="K69">
+        <v>227</v>
+      </c>
+      <c r="L69">
+        <v>168</v>
+      </c>
+      <c r="M69">
+        <v>185</v>
+      </c>
+      <c r="N69">
+        <v>147</v>
+      </c>
+      <c r="O69">
+        <v>180</v>
+      </c>
+      <c r="P69">
+        <v>105</v>
+      </c>
+      <c r="Q69">
+        <v>152</v>
+      </c>
+      <c r="R69">
+        <v>48</v>
+      </c>
+      <c r="S69">
+        <v>123</v>
+      </c>
+      <c r="T69">
+        <v>3</v>
+      </c>
+      <c r="U69">
+        <v>7</v>
+      </c>
+      <c r="V69">
+        <f t="shared" ref="V69" si="9">SUM(B69,D69,F69,H69,J69,L69,N69,P69,R69,T69)</f>
+        <v>1029</v>
+      </c>
+      <c r="W69">
+        <f t="shared" ref="W69" si="10">SUM(C69,E69,G69,I69,K69,M69,O69,Q69,S69,U69)</f>
+        <v>1647</v>
+      </c>
+      <c r="X69">
+        <f>(V69/(V69+W69))*100</f>
+        <v>38.45291479820628</v>
+      </c>
+      <c r="Y69">
+        <f>(W69/(V69+W69))*100</f>
+        <v>61.547085201793713</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update for 6/5-6/7
</commit_message>
<xml_diff>
--- a/coronadata_age_sex.xlsx
+++ b/coronadata_age_sex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvisc\Desktop\coronadata-local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED41D77-CA21-4514-9BAB-0018134B141E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE124B96-CE8D-44E0-A5C3-E3F33CF5DA14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -971,11 +971,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y79"/>
+  <dimension ref="A1:Y82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T83" sqref="T83"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V81" sqref="V81:Y82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7136,6 +7136,249 @@
       <c r="Y79">
         <f t="shared" ref="Y79" si="38">(W79/(V79+W79))*100</f>
         <v>61.56666666666667</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B80">
+        <v>57</v>
+      </c>
+      <c r="C80">
+        <v>86</v>
+      </c>
+      <c r="D80">
+        <v>132</v>
+      </c>
+      <c r="E80">
+        <v>304</v>
+      </c>
+      <c r="F80">
+        <v>161</v>
+      </c>
+      <c r="G80">
+        <v>269</v>
+      </c>
+      <c r="H80">
+        <v>123</v>
+      </c>
+      <c r="I80">
+        <v>225</v>
+      </c>
+      <c r="J80">
+        <v>181</v>
+      </c>
+      <c r="K80">
+        <v>258</v>
+      </c>
+      <c r="L80">
+        <v>184</v>
+      </c>
+      <c r="M80">
+        <v>202</v>
+      </c>
+      <c r="N80">
+        <v>159</v>
+      </c>
+      <c r="O80">
+        <v>189</v>
+      </c>
+      <c r="P80">
+        <v>115</v>
+      </c>
+      <c r="Q80">
+        <v>172</v>
+      </c>
+      <c r="R80">
+        <v>53</v>
+      </c>
+      <c r="S80">
+        <v>148</v>
+      </c>
+      <c r="T80">
+        <v>3</v>
+      </c>
+      <c r="U80">
+        <v>9</v>
+      </c>
+      <c r="V80">
+        <f t="shared" ref="V80" si="39">SUM(B80,D80,F80,H80,J80,L80,N80,P80,R80,T80)</f>
+        <v>1168</v>
+      </c>
+      <c r="W80">
+        <f t="shared" ref="W80" si="40">SUM(C80,E80,G80,I80,K80,M80,O80,Q80,S80,U80)</f>
+        <v>1862</v>
+      </c>
+      <c r="X80">
+        <f t="shared" ref="X80" si="41">(V80/(V80+W80))*100</f>
+        <v>38.547854785478549</v>
+      </c>
+      <c r="Y80">
+        <f t="shared" ref="Y80" si="42">(W80/(V80+W80))*100</f>
+        <v>61.452145214521451</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>43988</v>
+      </c>
+      <c r="B81">
+        <v>58</v>
+      </c>
+      <c r="C81">
+        <v>87</v>
+      </c>
+      <c r="D81">
+        <v>136</v>
+      </c>
+      <c r="E81">
+        <v>310</v>
+      </c>
+      <c r="F81">
+        <v>162</v>
+      </c>
+      <c r="G81">
+        <v>273</v>
+      </c>
+      <c r="H81">
+        <v>124</v>
+      </c>
+      <c r="I81">
+        <v>227</v>
+      </c>
+      <c r="J81">
+        <v>183</v>
+      </c>
+      <c r="K81">
+        <v>262</v>
+      </c>
+      <c r="L81">
+        <v>185</v>
+      </c>
+      <c r="M81">
+        <v>204</v>
+      </c>
+      <c r="N81">
+        <v>159</v>
+      </c>
+      <c r="O81">
+        <v>190</v>
+      </c>
+      <c r="P81">
+        <v>115</v>
+      </c>
+      <c r="Q81">
+        <v>172</v>
+      </c>
+      <c r="R81">
+        <v>53</v>
+      </c>
+      <c r="S81">
+        <v>150</v>
+      </c>
+      <c r="T81">
+        <v>3</v>
+      </c>
+      <c r="U81">
+        <v>9</v>
+      </c>
+      <c r="V81">
+        <f t="shared" ref="V81" si="43">SUM(B81,D81,F81,H81,J81,L81,N81,P81,R81,T81)</f>
+        <v>1178</v>
+      </c>
+      <c r="W81">
+        <f t="shared" ref="W81" si="44">SUM(C81,E81,G81,I81,K81,M81,O81,Q81,S81,U81)</f>
+        <v>1884</v>
+      </c>
+      <c r="X81">
+        <f t="shared" ref="X81" si="45">(V81/(V81+W81))*100</f>
+        <v>38.471587197909862</v>
+      </c>
+      <c r="Y81">
+        <f t="shared" ref="Y81" si="46">(W81/(V81+W81))*100</f>
+        <v>61.528412802090138</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>43989</v>
+      </c>
+      <c r="B82">
+        <v>60</v>
+      </c>
+      <c r="C82">
+        <v>88</v>
+      </c>
+      <c r="D82">
+        <v>137</v>
+      </c>
+      <c r="E82">
+        <v>314</v>
+      </c>
+      <c r="F82">
+        <v>164</v>
+      </c>
+      <c r="G82">
+        <v>275</v>
+      </c>
+      <c r="H82">
+        <v>124</v>
+      </c>
+      <c r="I82">
+        <v>231</v>
+      </c>
+      <c r="J82">
+        <v>186</v>
+      </c>
+      <c r="K82">
+        <v>263</v>
+      </c>
+      <c r="L82">
+        <v>185</v>
+      </c>
+      <c r="M82">
+        <v>206</v>
+      </c>
+      <c r="N82">
+        <v>159</v>
+      </c>
+      <c r="O82">
+        <v>191</v>
+      </c>
+      <c r="P82">
+        <v>115</v>
+      </c>
+      <c r="Q82">
+        <v>172</v>
+      </c>
+      <c r="R82">
+        <v>53</v>
+      </c>
+      <c r="S82">
+        <v>151</v>
+      </c>
+      <c r="T82">
+        <v>3</v>
+      </c>
+      <c r="U82">
+        <v>9</v>
+      </c>
+      <c r="V82">
+        <f t="shared" ref="V82" si="47">SUM(B82,D82,F82,H82,J82,L82,N82,P82,R82,T82)</f>
+        <v>1186</v>
+      </c>
+      <c r="W82">
+        <f t="shared" ref="W82" si="48">SUM(C82,E82,G82,I82,K82,M82,O82,Q82,S82,U82)</f>
+        <v>1900</v>
+      </c>
+      <c r="X82">
+        <f t="shared" ref="X82" si="49">(V82/(V82+W82))*100</f>
+        <v>38.431626701231366</v>
+      </c>
+      <c r="Y82">
+        <f t="shared" ref="Y82" si="50">(W82/(V82+W82))*100</f>
+        <v>61.568373298768634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>